<commit_message>
VBA: harcoded mock ready
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyu-homebase\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyu-homebase\repos\nab\build\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Features</t>
   </si>
@@ -84,6 +84,93 @@
   </si>
   <si>
     <t>random subscript error</t>
+  </si>
+  <si>
+    <t>cleanSheet</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>oh dear, why is my source data being manip?</t>
+  </si>
+  <si>
+    <t>sampleTest</t>
+  </si>
+  <si>
+    <t>loopRun</t>
+  </si>
+  <si>
+    <t>the rows delete incident</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>expo</t>
+  </si>
+  <si>
+    <t>expoGroup</t>
+  </si>
+  <si>
+    <t>col classes</t>
+  </si>
+  <si>
+    <t>title classes</t>
+  </si>
+  <si>
+    <t>object modelled better</t>
+  </si>
+  <si>
+    <t>sorting subroutines</t>
+  </si>
+  <si>
+    <t>Priority fillup</t>
+  </si>
+  <si>
+    <t>CCYgrouping</t>
+  </si>
+  <si>
+    <t>Tests..</t>
+  </si>
+  <si>
+    <t>update modules</t>
+  </si>
+  <si>
+    <t>temp, results sheets</t>
+  </si>
+  <si>
+    <t>Step class start</t>
+  </si>
+  <si>
+    <t>nah, just work with the groups</t>
+  </si>
+  <si>
+    <t>gaah, don't overload! Just worry about numbering in the objects</t>
+  </si>
+  <si>
+    <t>need to rubberduck the test modules.. A bit worrying as the sphegetti code gets larger</t>
+  </si>
+  <si>
+    <t>create the sheets independantly</t>
+  </si>
+  <si>
+    <t>modularize the variables.. And call them from the autogenerated code</t>
+  </si>
+  <si>
+    <t>indep sheet creation</t>
+  </si>
+  <si>
+    <t>pending: compute all other results</t>
+  </si>
+  <si>
+    <t>pending: compute HCs properly</t>
+  </si>
+  <si>
+    <t>pending: discuss with tech the fields</t>
   </si>
 </sst>
 </file>
@@ -119,8 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,105 +526,268 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="61.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.21875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="36.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>0.18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>0.21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>0.22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E22" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VBA: may have just cracked it
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Features</t>
   </si>
@@ -171,6 +171,33 @@
   </si>
   <si>
     <t>pending: discuss with tech the fields</t>
+  </si>
+  <si>
+    <t>Decider started</t>
+  </si>
+  <si>
+    <t>mapping on progress</t>
+  </si>
+  <si>
+    <t>decider.inform status.. Need to read the types and load collections</t>
+  </si>
+  <si>
+    <t>more on the decider</t>
+  </si>
+  <si>
+    <t>constants updated with flags and tags</t>
+  </si>
+  <si>
+    <t>consumtion module connected</t>
+  </si>
+  <si>
+    <t>clean up on non-dry code.. More comments in the decider</t>
+  </si>
+  <si>
+    <t>cleaned up old modules</t>
+  </si>
+  <si>
+    <t>may have just cracked consumption</t>
   </si>
 </sst>
 </file>
@@ -526,11 +553,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,6 +817,49 @@
         <v>48</v>
       </c>
     </row>
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
VBA: ready for beta-testing
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Features</t>
   </si>
@@ -198,6 +198,27 @@
   </si>
   <si>
     <t>may have just cracked consumption</t>
+  </si>
+  <si>
+    <t>seemed like the CCY works fine.. But say some errors on random testing though</t>
+  </si>
+  <si>
+    <t>NMS priorit for consumption</t>
+  </si>
+  <si>
+    <t>wait, there seems to be no bugs here.. Lets see what assumptions are broken in her rand test</t>
+  </si>
+  <si>
+    <t>Signoff</t>
+  </si>
+  <si>
+    <t>Proper ordering</t>
+  </si>
+  <si>
+    <t>Comment status message</t>
+  </si>
+  <si>
+    <t>better PE MS group naming</t>
   </si>
 </sst>
 </file>
@@ -553,11 +574,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,7 +852,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>0.26</v>
       </c>
@@ -840,6 +861,9 @@
       </c>
       <c r="C28" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -858,6 +882,33 @@
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VBA: need for optimization
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Features</t>
   </si>
@@ -228,6 +228,33 @@
   </si>
   <si>
     <t>think about every step outputting..</t>
+  </si>
+  <si>
+    <t>just updating with 'the magic button' to show the result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input CCY sorting based on </t>
+  </si>
+  <si>
+    <t>PERC, NPERC</t>
+  </si>
+  <si>
+    <t>Availability calc properly</t>
+  </si>
+  <si>
+    <t>cons order grouping issue</t>
+  </si>
+  <si>
+    <t>HC selection automation</t>
+  </si>
+  <si>
+    <t>freeze panes on autosort</t>
+  </si>
+  <si>
+    <t>cons per expos if needed</t>
+  </si>
+  <si>
+    <t>dec sum remainings</t>
   </si>
 </sst>
 </file>
@@ -583,11 +610,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,7 +934,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
@@ -915,12 +942,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>0.28000000000000003</v>
       </c>
@@ -931,9 +958,54 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D36" s="1" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VBA: 0.30 release, ready for beta testing
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="manual"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>Features</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>dec sum remainings</t>
+  </si>
+  <si>
+    <t>noticing some performance hits, need to profile sometime</t>
   </si>
 </sst>
 </file>
@@ -610,11 +613,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +937,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
@@ -942,12 +945,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>0.28000000000000003</v>
       </c>
@@ -958,12 +961,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D36" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>0.28999999999999998</v>
       </c>
@@ -971,7 +974,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>0.3</v>
       </c>
@@ -981,31 +984,35 @@
       <c r="C38" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="D38" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="E38" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="D39" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VBA: semi done step results
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>Features</t>
   </si>
@@ -258,6 +258,54 @@
   </si>
   <si>
     <t>noticing some performance hits, need to profile sometime</t>
+  </si>
+  <si>
+    <t>More examples</t>
+  </si>
+  <si>
+    <t>Disabling events for more optimization</t>
+  </si>
+  <si>
+    <t>NPE alone logic fix</t>
+  </si>
+  <si>
+    <t>NPE logic change based on brd</t>
+  </si>
+  <si>
+    <t>consider updating the one cell alone, need to optimize</t>
+  </si>
+  <si>
+    <t>doing some terrible hacking for the sort method, need to see if this can be done better</t>
+  </si>
+  <si>
+    <t>Feature requests: print all the steps, descriptions needed for the different columns</t>
+  </si>
+  <si>
+    <t>task to add the col descs</t>
+  </si>
+  <si>
+    <t>investigate the activewindow FreezePane error</t>
+  </si>
+  <si>
+    <t>moved steps up to have it be the first sheet</t>
+  </si>
+  <si>
+    <t>optimized assets</t>
+  </si>
+  <si>
+    <t>need to do the same optim for expos</t>
+  </si>
+  <si>
+    <t>renamed sheet names and stuff</t>
+  </si>
+  <si>
+    <t>need to write out steps</t>
+  </si>
+  <si>
+    <t>freezePain optimization</t>
+  </si>
+  <si>
+    <t>need to write out reasons</t>
   </si>
 </sst>
 </file>
@@ -613,20 +661,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="41" style="1" customWidth="1"/>
     <col min="4" max="4" width="41.21875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="36.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -1014,6 +1063,73 @@
       <c r="A41" s="1">
         <v>0.31</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DS: adding myDataStructures classes
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyu-homebase\repos\nab\build\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="v0" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
   <si>
     <t>Features</t>
   </si>
@@ -341,12 +346,15 @@
   </si>
   <si>
     <t>need to build arrangement sort logic as well</t>
+  </si>
+  <si>
+    <t>Adding myGraph, myStack, myQueue, mySet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -687,7 +695,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -703,18 +711,18 @@
       <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="30.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="41" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.7</v>
       </c>
@@ -739,7 +747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.8</v>
       </c>
@@ -747,7 +755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.9</v>
       </c>
@@ -758,7 +766,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
@@ -766,7 +774,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.11</v>
       </c>
@@ -774,7 +782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.12</v>
       </c>
@@ -785,7 +793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.13</v>
       </c>
@@ -793,7 +801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.14000000000000001</v>
       </c>
@@ -801,7 +809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.15</v>
       </c>
@@ -809,12 +817,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.16</v>
       </c>
@@ -825,12 +833,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
@@ -838,7 +846,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.17</v>
       </c>
@@ -846,7 +854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0.18</v>
       </c>
@@ -857,17 +865,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0.21</v>
       </c>
@@ -884,7 +892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
@@ -895,7 +903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.22</v>
       </c>
@@ -912,7 +920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
@@ -923,7 +931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.23</v>
       </c>
@@ -934,7 +942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>0.24</v>
       </c>
@@ -948,7 +956,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
@@ -956,12 +964,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E26" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>0.25</v>
       </c>
@@ -975,7 +983,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>0.26</v>
       </c>
@@ -989,7 +997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>53</v>
       </c>
@@ -997,17 +1005,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>0.27</v>
       </c>
@@ -1021,7 +1029,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
@@ -1029,12 +1037,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>0.28000000000000003</v>
       </c>
@@ -1045,12 +1053,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D36" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>0.28999999999999998</v>
       </c>
@@ -1058,7 +1066,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>0.3</v>
       </c>
@@ -1078,7 +1086,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>74</v>
       </c>
@@ -1089,12 +1097,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>0.31</v>
       </c>
@@ -1105,7 +1113,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>0.32</v>
       </c>
@@ -1122,7 +1130,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>0.33</v>
       </c>
@@ -1133,7 +1141,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>0.34</v>
       </c>
@@ -1150,7 +1158,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>90</v>
       </c>
@@ -1158,7 +1166,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1166,7 +1174,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>0.35</v>
       </c>
@@ -1174,7 +1182,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>0.36</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>0.37</v>
       </c>
@@ -1190,7 +1198,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>0.38</v>
       </c>
@@ -1198,7 +1206,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>0.39</v>
       </c>
@@ -1206,7 +1214,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>0.4</v>
       </c>
@@ -1214,7 +1222,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>0.41</v>
       </c>
@@ -1225,7 +1233,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>0.42</v>
       </c>
@@ -1239,21 +1247,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
@@ -1273,7 +1281,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.01</v>
       </c>
@@ -1288,6 +1296,14 @@
       </c>
       <c r="E2" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1.02</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XLS: 1.04 with changeLog update
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t>Features</t>
   </si>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>Adding myGraph, myStack, myQueue, mySet</t>
+  </si>
+  <si>
+    <t>cleaning up the assets mod</t>
+  </si>
+  <si>
+    <t>logger enhancement</t>
+  </si>
+  <si>
+    <t>pledges setup</t>
+  </si>
+  <si>
+    <t>arrangements setup</t>
   </si>
 </sst>
 </file>
@@ -1247,10 +1259,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1306,6 +1318,30 @@
         <v>107</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1.03</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1.04</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
XLS: started the addition and logger changes
</commit_message>
<xml_diff>
--- a/build/Consumer-ChangeLog.xlsx
+++ b/build/Consumer-ChangeLog.xlsx
@@ -16,6 +16,7 @@
     <sheet name="v1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>Features</t>
   </si>
@@ -361,6 +362,15 @@
   </si>
   <si>
     <t>arrangements setup</t>
+  </si>
+  <si>
+    <t>Logger trace level added</t>
+  </si>
+  <si>
+    <t>pledge read</t>
+  </si>
+  <si>
+    <t>arrangement read</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1269,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,6 +1352,22 @@
         <v>111</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1.05</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>